<commit_message>
Test prve promene na .xlsx fajlu
</commit_message>
<xml_diff>
--- a/F2-Budget.xlsx
+++ b/F2-Budget.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5472BBFD-F64B-44F0-9A37-179486FBEE7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C30D2BF-3248-4C57-A006-73F167DD7ACB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1065,7 +1065,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1112,6 +1112,18 @@
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1410,7 +1422,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="220">
+  <cellXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1771,6 +1783,167 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1789,32 +1962,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1857,140 +2004,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1998,47 +2019,29 @@
     <xf numFmtId="0" fontId="18" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2057,18 +2060,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -2089,6 +2080,33 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2469,7 +2487,7 @@
   <dimension ref="A1:Q144"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A2" sqref="A2:O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2490,59 +2508,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="154" t="s">
+      <c r="A1" s="220" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="154"/>
-      <c r="C1" s="154"/>
-      <c r="D1" s="154"/>
-      <c r="E1" s="154"/>
-      <c r="F1" s="154"/>
-      <c r="G1" s="154"/>
-      <c r="H1" s="154"/>
-      <c r="I1" s="154"/>
-      <c r="J1" s="154"/>
-      <c r="K1" s="154"/>
-      <c r="L1" s="154"/>
-      <c r="M1" s="154"/>
-      <c r="N1" s="154"/>
-      <c r="O1" s="154"/>
+      <c r="B1" s="220"/>
+      <c r="C1" s="220"/>
+      <c r="D1" s="220"/>
+      <c r="E1" s="220"/>
+      <c r="F1" s="220"/>
+      <c r="G1" s="220"/>
+      <c r="H1" s="220"/>
+      <c r="I1" s="220"/>
+      <c r="J1" s="220"/>
+      <c r="K1" s="220"/>
+      <c r="L1" s="220"/>
+      <c r="M1" s="220"/>
+      <c r="N1" s="220"/>
+      <c r="O1" s="220"/>
     </row>
     <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="155" t="s">
+      <c r="A2" s="221" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="155"/>
-      <c r="C2" s="155"/>
-      <c r="D2" s="155"/>
-      <c r="E2" s="155"/>
-      <c r="F2" s="155"/>
-      <c r="G2" s="155"/>
-      <c r="H2" s="155"/>
-      <c r="I2" s="155"/>
-      <c r="J2" s="155"/>
-      <c r="K2" s="155"/>
-      <c r="L2" s="155"/>
-      <c r="M2" s="155"/>
-      <c r="N2" s="155"/>
-      <c r="O2" s="155"/>
+      <c r="B2" s="221"/>
+      <c r="C2" s="221"/>
+      <c r="D2" s="221"/>
+      <c r="E2" s="221"/>
+      <c r="F2" s="221"/>
+      <c r="G2" s="221"/>
+      <c r="H2" s="221"/>
+      <c r="I2" s="221"/>
+      <c r="J2" s="221"/>
+      <c r="K2" s="221"/>
+      <c r="L2" s="221"/>
+      <c r="M2" s="221"/>
+      <c r="N2" s="221"/>
+      <c r="O2" s="221"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="156"/>
-      <c r="B3" s="156"/>
-      <c r="C3" s="156"/>
-      <c r="D3" s="156"/>
-      <c r="E3" s="156"/>
-      <c r="F3" s="156"/>
-      <c r="G3" s="156"/>
-      <c r="H3" s="156"/>
-      <c r="I3" s="156"/>
-      <c r="J3" s="156"/>
-      <c r="K3" s="156"/>
-      <c r="L3" s="156"/>
-      <c r="M3" s="156"/>
-      <c r="N3" s="156"/>
-      <c r="O3" s="156"/>
+      <c r="A3" s="144"/>
+      <c r="B3" s="144"/>
+      <c r="C3" s="144"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+      <c r="H3" s="144"/>
+      <c r="I3" s="144"/>
+      <c r="J3" s="144"/>
+      <c r="K3" s="144"/>
+      <c r="L3" s="144"/>
+      <c r="M3" s="144"/>
+      <c r="N3" s="144"/>
+      <c r="O3" s="144"/>
     </row>
     <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
@@ -2562,31 +2580,31 @@
       <c r="O4" s="6"/>
     </row>
     <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="152" t="s">
+      <c r="A5" s="166" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="153"/>
-      <c r="C5" s="157" t="s">
+      <c r="B5" s="167"/>
+      <c r="C5" s="145" t="s">
         <v>118</v>
       </c>
-      <c r="D5" s="158"/>
-      <c r="E5" s="158"/>
-      <c r="F5" s="158"/>
-      <c r="G5" s="158"/>
-      <c r="H5" s="158"/>
-      <c r="I5" s="158"/>
-      <c r="J5" s="158"/>
-      <c r="K5" s="158"/>
-      <c r="L5" s="158"/>
-      <c r="M5" s="158"/>
-      <c r="N5" s="158"/>
-      <c r="O5" s="159"/>
+      <c r="D5" s="146"/>
+      <c r="E5" s="146"/>
+      <c r="F5" s="146"/>
+      <c r="G5" s="146"/>
+      <c r="H5" s="146"/>
+      <c r="I5" s="146"/>
+      <c r="J5" s="146"/>
+      <c r="K5" s="146"/>
+      <c r="L5" s="146"/>
+      <c r="M5" s="146"/>
+      <c r="N5" s="146"/>
+      <c r="O5" s="147"/>
     </row>
     <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="152" t="s">
+      <c r="A6" s="166" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="153"/>
+      <c r="B6" s="167"/>
       <c r="C6" s="7"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
@@ -2604,46 +2622,46 @@
       <c r="O6" s="9"/>
     </row>
     <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="152" t="s">
+      <c r="A7" s="166" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="153"/>
-      <c r="C7" s="157" t="s">
+      <c r="B7" s="167"/>
+      <c r="C7" s="145" t="s">
         <v>120</v>
       </c>
-      <c r="D7" s="158"/>
-      <c r="E7" s="158"/>
-      <c r="F7" s="158"/>
-      <c r="G7" s="158"/>
-      <c r="H7" s="158"/>
-      <c r="I7" s="158"/>
-      <c r="J7" s="158"/>
-      <c r="K7" s="158"/>
-      <c r="L7" s="158"/>
-      <c r="M7" s="158"/>
-      <c r="N7" s="158"/>
-      <c r="O7" s="159"/>
+      <c r="D7" s="146"/>
+      <c r="E7" s="146"/>
+      <c r="F7" s="146"/>
+      <c r="G7" s="146"/>
+      <c r="H7" s="146"/>
+      <c r="I7" s="146"/>
+      <c r="J7" s="146"/>
+      <c r="K7" s="146"/>
+      <c r="L7" s="146"/>
+      <c r="M7" s="146"/>
+      <c r="N7" s="146"/>
+      <c r="O7" s="147"/>
     </row>
     <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="152" t="s">
+      <c r="A8" s="166" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="153"/>
-      <c r="C8" s="157" t="s">
+      <c r="B8" s="167"/>
+      <c r="C8" s="145" t="s">
         <v>121</v>
       </c>
-      <c r="D8" s="158"/>
-      <c r="E8" s="158"/>
-      <c r="F8" s="158"/>
-      <c r="G8" s="158"/>
-      <c r="H8" s="158"/>
-      <c r="I8" s="158"/>
-      <c r="J8" s="158"/>
-      <c r="K8" s="158"/>
-      <c r="L8" s="158"/>
-      <c r="M8" s="158"/>
-      <c r="N8" s="158"/>
-      <c r="O8" s="159"/>
+      <c r="D8" s="146"/>
+      <c r="E8" s="146"/>
+      <c r="F8" s="146"/>
+      <c r="G8" s="146"/>
+      <c r="H8" s="146"/>
+      <c r="I8" s="146"/>
+      <c r="J8" s="146"/>
+      <c r="K8" s="146"/>
+      <c r="L8" s="146"/>
+      <c r="M8" s="146"/>
+      <c r="N8" s="146"/>
+      <c r="O8" s="147"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C9" s="6"/>
@@ -2691,14 +2709,14 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
-      <c r="J11" s="118" t="s">
+      <c r="J11" s="170" t="s">
         <v>59</v>
       </c>
-      <c r="K11" s="119"/>
-      <c r="L11" s="119"/>
-      <c r="M11" s="119"/>
-      <c r="N11" s="119"/>
-      <c r="O11" s="120"/>
+      <c r="K11" s="171"/>
+      <c r="L11" s="171"/>
+      <c r="M11" s="171"/>
+      <c r="N11" s="171"/>
+      <c r="O11" s="172"/>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -2716,14 +2734,14 @@
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
-      <c r="J12" s="118" t="s">
+      <c r="J12" s="170" t="s">
         <v>61</v>
       </c>
-      <c r="K12" s="119"/>
-      <c r="L12" s="119"/>
-      <c r="M12" s="119"/>
-      <c r="N12" s="119"/>
-      <c r="O12" s="120"/>
+      <c r="K12" s="171"/>
+      <c r="L12" s="171"/>
+      <c r="M12" s="171"/>
+      <c r="N12" s="171"/>
+      <c r="O12" s="172"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
@@ -2743,65 +2761,65 @@
       <c r="O13" s="6"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="134" t="s">
+      <c r="A14" s="178" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="135"/>
-      <c r="C14" s="135"/>
-      <c r="D14" s="135"/>
-      <c r="E14" s="135"/>
-      <c r="F14" s="135"/>
-      <c r="G14" s="135"/>
-      <c r="H14" s="135"/>
-      <c r="I14" s="135"/>
-      <c r="J14" s="135"/>
-      <c r="K14" s="135"/>
-      <c r="L14" s="135"/>
-      <c r="M14" s="135"/>
-      <c r="N14" s="135"/>
-      <c r="O14" s="136"/>
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="179"/>
+      <c r="E14" s="179"/>
+      <c r="F14" s="179"/>
+      <c r="G14" s="179"/>
+      <c r="H14" s="179"/>
+      <c r="I14" s="179"/>
+      <c r="J14" s="179"/>
+      <c r="K14" s="179"/>
+      <c r="L14" s="179"/>
+      <c r="M14" s="179"/>
+      <c r="N14" s="179"/>
+      <c r="O14" s="180"/>
     </row>
     <row r="15" spans="1:15" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="129" t="s">
+      <c r="A15" s="134" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="145" t="s">
+      <c r="B15" s="159" t="s">
         <v>107</v>
       </c>
-      <c r="C15" s="129" t="s">
+      <c r="C15" s="134" t="s">
         <v>106</v>
       </c>
-      <c r="D15" s="141" t="s">
+      <c r="D15" s="185" t="s">
         <v>108</v>
       </c>
-      <c r="E15" s="142"/>
-      <c r="F15" s="137" t="s">
+      <c r="E15" s="186"/>
+      <c r="F15" s="181" t="s">
         <v>102</v>
       </c>
-      <c r="G15" s="138"/>
-      <c r="H15" s="131" t="s">
+      <c r="G15" s="182"/>
+      <c r="H15" s="175" t="s">
         <v>100</v>
       </c>
-      <c r="I15" s="132"/>
-      <c r="J15" s="133"/>
+      <c r="I15" s="176"/>
+      <c r="J15" s="177"/>
       <c r="K15" s="92" t="s">
         <v>99</v>
       </c>
-      <c r="L15" s="137" t="s">
+      <c r="L15" s="181" t="s">
         <v>101</v>
       </c>
-      <c r="M15" s="138"/>
-      <c r="N15" s="139" t="s">
+      <c r="M15" s="182"/>
+      <c r="N15" s="183" t="s">
         <v>35</v>
       </c>
-      <c r="O15" s="140"/>
+      <c r="O15" s="184"/>
     </row>
     <row r="16" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="130"/>
-      <c r="B16" s="146"/>
-      <c r="C16" s="130"/>
-      <c r="D16" s="143"/>
-      <c r="E16" s="144"/>
+      <c r="A16" s="135"/>
+      <c r="B16" s="160"/>
+      <c r="C16" s="135"/>
+      <c r="D16" s="187"/>
+      <c r="E16" s="188"/>
       <c r="F16" s="89" t="s">
         <v>7</v>
       </c>
@@ -2843,10 +2861,10 @@
       <c r="C17" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="D17" s="121" t="s">
+      <c r="D17" s="173" t="s">
         <v>141</v>
       </c>
-      <c r="E17" s="122"/>
+      <c r="E17" s="174"/>
       <c r="F17" s="90">
         <v>49500</v>
       </c>
@@ -2894,10 +2912,10 @@
       <c r="C18" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="D18" s="123" t="s">
+      <c r="D18" s="168" t="s">
         <v>142</v>
       </c>
-      <c r="E18" s="124"/>
+      <c r="E18" s="169"/>
       <c r="F18" s="90">
         <v>38750</v>
       </c>
@@ -2945,10 +2963,10 @@
       <c r="C19" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="D19" s="123" t="s">
+      <c r="D19" s="168" t="s">
         <v>142</v>
       </c>
-      <c r="E19" s="124"/>
+      <c r="E19" s="169"/>
       <c r="F19" s="90">
         <v>38750</v>
       </c>
@@ -2996,10 +3014,10 @@
       <c r="C20" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="D20" s="123" t="s">
+      <c r="D20" s="168" t="s">
         <v>143</v>
       </c>
-      <c r="E20" s="124"/>
+      <c r="E20" s="169"/>
       <c r="F20" s="90">
         <v>42000</v>
       </c>
@@ -3047,10 +3065,10 @@
       <c r="C21" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="D21" s="123" t="s">
+      <c r="D21" s="168" t="s">
         <v>144</v>
       </c>
-      <c r="E21" s="124"/>
+      <c r="E21" s="169"/>
       <c r="F21" s="90">
         <v>41250</v>
       </c>
@@ -3097,10 +3115,10 @@
       <c r="C22" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="D22" s="123" t="s">
+      <c r="D22" s="168" t="s">
         <v>145</v>
       </c>
-      <c r="E22" s="124"/>
+      <c r="E22" s="169"/>
       <c r="F22" s="90">
         <v>31000</v>
       </c>
@@ -3148,10 +3166,10 @@
       <c r="C23" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="D23" s="123" t="s">
+      <c r="D23" s="168" t="s">
         <v>146</v>
       </c>
-      <c r="E23" s="124"/>
+      <c r="E23" s="169"/>
       <c r="F23" s="90">
         <v>42000</v>
       </c>
@@ -3198,10 +3216,10 @@
       <c r="C24" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="D24" s="123" t="s">
+      <c r="D24" s="168" t="s">
         <v>147</v>
       </c>
-      <c r="E24" s="124"/>
+      <c r="E24" s="169"/>
       <c r="F24" s="90">
         <v>36000</v>
       </c>
@@ -3248,10 +3266,10 @@
       <c r="C25" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="D25" s="123" t="s">
+      <c r="D25" s="168" t="s">
         <v>144</v>
       </c>
-      <c r="E25" s="124"/>
+      <c r="E25" s="169"/>
       <c r="F25" s="90">
         <v>33000</v>
       </c>
@@ -3298,10 +3316,10 @@
       <c r="C26" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D26" s="123" t="s">
+      <c r="D26" s="168" t="s">
         <v>144</v>
       </c>
-      <c r="E26" s="124"/>
+      <c r="E26" s="169"/>
       <c r="F26" s="90">
         <v>41250</v>
       </c>
@@ -3348,10 +3366,10 @@
       <c r="C27" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="D27" s="123" t="s">
+      <c r="D27" s="168" t="s">
         <v>147</v>
       </c>
-      <c r="E27" s="124"/>
+      <c r="E27" s="169"/>
       <c r="F27" s="90">
         <v>36000</v>
       </c>
@@ -3398,10 +3416,10 @@
       <c r="C28" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="D28" s="123" t="s">
+      <c r="D28" s="168" t="s">
         <v>148</v>
       </c>
-      <c r="E28" s="124"/>
+      <c r="E28" s="169"/>
       <c r="F28" s="90">
         <v>33000</v>
       </c>
@@ -3439,14 +3457,14 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="126" t="s">
+      <c r="A29" s="118" t="s">
         <v>75</v>
       </c>
-      <c r="B29" s="127"/>
-      <c r="C29" s="127"/>
-      <c r="D29" s="127"/>
-      <c r="E29" s="127"/>
-      <c r="F29" s="127"/>
+      <c r="B29" s="119"/>
+      <c r="C29" s="119"/>
+      <c r="D29" s="119"/>
+      <c r="E29" s="119"/>
+      <c r="F29" s="119"/>
       <c r="G29" s="54" t="s">
         <v>17</v>
       </c>
@@ -3514,50 +3532,50 @@
       <c r="O31" s="6"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A32" s="128" t="s">
+      <c r="A32" s="123" t="s">
         <v>94</v>
       </c>
-      <c r="B32" s="128"/>
-      <c r="C32" s="128"/>
-      <c r="D32" s="128"/>
-      <c r="E32" s="128"/>
-      <c r="F32" s="128"/>
-      <c r="G32" s="128"/>
-      <c r="H32" s="128"/>
-      <c r="I32" s="128"/>
-      <c r="J32" s="128"/>
-      <c r="K32" s="128"/>
-      <c r="L32" s="128"/>
-      <c r="M32" s="128"/>
-      <c r="N32" s="128"/>
-      <c r="O32" s="128"/>
+      <c r="B32" s="123"/>
+      <c r="C32" s="123"/>
+      <c r="D32" s="123"/>
+      <c r="E32" s="123"/>
+      <c r="F32" s="123"/>
+      <c r="G32" s="123"/>
+      <c r="H32" s="123"/>
+      <c r="I32" s="123"/>
+      <c r="J32" s="123"/>
+      <c r="K32" s="123"/>
+      <c r="L32" s="123"/>
+      <c r="M32" s="123"/>
+      <c r="N32" s="123"/>
+      <c r="O32" s="123"/>
     </row>
     <row r="33" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="175" t="s">
+      <c r="A33" s="121" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="129" t="s">
+      <c r="B33" s="134" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="151" t="s">
+      <c r="C33" s="165" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="188" t="s">
+      <c r="D33" s="124" t="s">
         <v>18</v>
       </c>
-      <c r="E33" s="147" t="s">
+      <c r="E33" s="161" t="s">
         <v>44</v>
       </c>
-      <c r="F33" s="148"/>
-      <c r="G33" s="148"/>
-      <c r="H33" s="148"/>
-      <c r="I33" s="148"/>
-      <c r="J33" s="148"/>
-      <c r="K33" s="125" t="s">
+      <c r="F33" s="162"/>
+      <c r="G33" s="162"/>
+      <c r="H33" s="162"/>
+      <c r="I33" s="162"/>
+      <c r="J33" s="162"/>
+      <c r="K33" s="133" t="s">
         <v>15</v>
       </c>
-      <c r="L33" s="125"/>
-      <c r="M33" s="125"/>
+      <c r="L33" s="133"/>
+      <c r="M33" s="133"/>
       <c r="N33" s="31" t="s">
         <v>15</v>
       </c>
@@ -3566,16 +3584,16 @@
       </c>
     </row>
     <row r="34" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="176"/>
-      <c r="B34" s="130"/>
-      <c r="C34" s="151"/>
-      <c r="D34" s="188"/>
-      <c r="E34" s="149"/>
-      <c r="F34" s="150"/>
-      <c r="G34" s="150"/>
-      <c r="H34" s="150"/>
-      <c r="I34" s="150"/>
-      <c r="J34" s="150"/>
+      <c r="A34" s="122"/>
+      <c r="B34" s="135"/>
+      <c r="C34" s="165"/>
+      <c r="D34" s="124"/>
+      <c r="E34" s="163"/>
+      <c r="F34" s="164"/>
+      <c r="G34" s="164"/>
+      <c r="H34" s="164"/>
+      <c r="I34" s="164"/>
+      <c r="J34" s="164"/>
       <c r="K34" s="80" t="s">
         <v>23</v>
       </c>
@@ -3585,10 +3603,10 @@
       <c r="M34" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="N34" s="166" t="s">
+      <c r="N34" s="125" t="s">
         <v>22</v>
       </c>
-      <c r="O34" s="167"/>
+      <c r="O34" s="126"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="32">
@@ -4302,17 +4320,17 @@
       </c>
     </row>
     <row r="53" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="127" t="s">
+      <c r="A53" s="119" t="s">
         <v>75</v>
       </c>
-      <c r="B53" s="127"/>
-      <c r="C53" s="127"/>
-      <c r="D53" s="127"/>
-      <c r="E53" s="127"/>
-      <c r="F53" s="127"/>
-      <c r="G53" s="127"/>
-      <c r="H53" s="127"/>
-      <c r="I53" s="127"/>
+      <c r="B53" s="119"/>
+      <c r="C53" s="119"/>
+      <c r="D53" s="119"/>
+      <c r="E53" s="119"/>
+      <c r="F53" s="119"/>
+      <c r="G53" s="119"/>
+      <c r="H53" s="119"/>
+      <c r="I53" s="119"/>
       <c r="J53" s="108" t="s">
         <v>17</v>
       </c>
@@ -4389,48 +4407,48 @@
       <c r="O56" s="6"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A57" s="128" t="s">
+      <c r="A57" s="123" t="s">
         <v>95</v>
       </c>
-      <c r="B57" s="128"/>
-      <c r="C57" s="128"/>
-      <c r="D57" s="128"/>
-      <c r="E57" s="128"/>
-      <c r="F57" s="128"/>
-      <c r="G57" s="128"/>
-      <c r="H57" s="128"/>
-      <c r="I57" s="128"/>
-      <c r="J57" s="128"/>
-      <c r="K57" s="128"/>
-      <c r="L57" s="128"/>
-      <c r="M57" s="128"/>
-      <c r="N57" s="128"/>
-      <c r="O57" s="128"/>
+      <c r="B57" s="123"/>
+      <c r="C57" s="123"/>
+      <c r="D57" s="123"/>
+      <c r="E57" s="123"/>
+      <c r="F57" s="123"/>
+      <c r="G57" s="123"/>
+      <c r="H57" s="123"/>
+      <c r="I57" s="123"/>
+      <c r="J57" s="123"/>
+      <c r="K57" s="123"/>
+      <c r="L57" s="123"/>
+      <c r="M57" s="123"/>
+      <c r="N57" s="123"/>
+      <c r="O57" s="123"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A58" s="175" t="s">
+      <c r="A58" s="121" t="s">
         <v>36</v>
       </c>
-      <c r="B58" s="129" t="s">
+      <c r="B58" s="134" t="s">
         <v>52</v>
       </c>
-      <c r="C58" s="129" t="s">
+      <c r="C58" s="134" t="s">
         <v>32</v>
       </c>
-      <c r="D58" s="182" t="s">
+      <c r="D58" s="127" t="s">
         <v>40</v>
       </c>
-      <c r="E58" s="183"/>
-      <c r="F58" s="183"/>
-      <c r="G58" s="183"/>
-      <c r="H58" s="183"/>
-      <c r="I58" s="183"/>
-      <c r="J58" s="184"/>
-      <c r="K58" s="125" t="s">
+      <c r="E58" s="128"/>
+      <c r="F58" s="128"/>
+      <c r="G58" s="128"/>
+      <c r="H58" s="128"/>
+      <c r="I58" s="128"/>
+      <c r="J58" s="129"/>
+      <c r="K58" s="133" t="s">
         <v>15</v>
       </c>
-      <c r="L58" s="125"/>
-      <c r="M58" s="125"/>
+      <c r="L58" s="133"/>
+      <c r="M58" s="133"/>
       <c r="N58" s="31" t="s">
         <v>15</v>
       </c>
@@ -4439,16 +4457,16 @@
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A59" s="176"/>
-      <c r="B59" s="130"/>
-      <c r="C59" s="130"/>
-      <c r="D59" s="185"/>
-      <c r="E59" s="186"/>
-      <c r="F59" s="186"/>
-      <c r="G59" s="186"/>
-      <c r="H59" s="186"/>
-      <c r="I59" s="186"/>
-      <c r="J59" s="187"/>
+      <c r="A59" s="122"/>
+      <c r="B59" s="135"/>
+      <c r="C59" s="135"/>
+      <c r="D59" s="130"/>
+      <c r="E59" s="131"/>
+      <c r="F59" s="131"/>
+      <c r="G59" s="131"/>
+      <c r="H59" s="131"/>
+      <c r="I59" s="131"/>
+      <c r="J59" s="132"/>
       <c r="K59" s="80" t="s">
         <v>23</v>
       </c>
@@ -4458,10 +4476,10 @@
       <c r="M59" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="N59" s="166" t="s">
+      <c r="N59" s="125" t="s">
         <v>22</v>
       </c>
-      <c r="O59" s="167"/>
+      <c r="O59" s="126"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="32">
@@ -4785,17 +4803,17 @@
       </c>
     </row>
     <row r="69" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="126" t="s">
+      <c r="A69" s="118" t="s">
         <v>75</v>
       </c>
-      <c r="B69" s="127"/>
-      <c r="C69" s="127"/>
-      <c r="D69" s="127"/>
-      <c r="E69" s="127"/>
-      <c r="F69" s="127"/>
-      <c r="G69" s="127"/>
-      <c r="H69" s="127"/>
-      <c r="I69" s="171"/>
+      <c r="B69" s="119"/>
+      <c r="C69" s="119"/>
+      <c r="D69" s="119"/>
+      <c r="E69" s="119"/>
+      <c r="F69" s="119"/>
+      <c r="G69" s="119"/>
+      <c r="H69" s="119"/>
+      <c r="I69" s="120"/>
       <c r="J69" s="54" t="s">
         <v>17</v>
       </c>
@@ -4869,48 +4887,48 @@
       <c r="O72" s="6"/>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A73" s="128" t="s">
+      <c r="A73" s="123" t="s">
         <v>19</v>
       </c>
-      <c r="B73" s="128"/>
-      <c r="C73" s="128"/>
-      <c r="D73" s="128"/>
-      <c r="E73" s="128"/>
-      <c r="F73" s="128"/>
-      <c r="G73" s="128"/>
-      <c r="H73" s="128"/>
-      <c r="I73" s="128"/>
-      <c r="J73" s="128"/>
-      <c r="K73" s="128"/>
-      <c r="L73" s="128"/>
-      <c r="M73" s="128"/>
-      <c r="N73" s="128"/>
-      <c r="O73" s="128"/>
+      <c r="B73" s="123"/>
+      <c r="C73" s="123"/>
+      <c r="D73" s="123"/>
+      <c r="E73" s="123"/>
+      <c r="F73" s="123"/>
+      <c r="G73" s="123"/>
+      <c r="H73" s="123"/>
+      <c r="I73" s="123"/>
+      <c r="J73" s="123"/>
+      <c r="K73" s="123"/>
+      <c r="L73" s="123"/>
+      <c r="M73" s="123"/>
+      <c r="N73" s="123"/>
+      <c r="O73" s="123"/>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A74" s="175" t="s">
+      <c r="A74" s="121" t="s">
         <v>36</v>
       </c>
-      <c r="B74" s="129" t="s">
+      <c r="B74" s="134" t="s">
         <v>52</v>
       </c>
-      <c r="C74" s="165" t="s">
+      <c r="C74" s="137" t="s">
         <v>76</v>
       </c>
-      <c r="D74" s="182" t="s">
+      <c r="D74" s="127" t="s">
         <v>77</v>
       </c>
-      <c r="E74" s="183"/>
-      <c r="F74" s="183"/>
-      <c r="G74" s="183"/>
-      <c r="H74" s="183"/>
-      <c r="I74" s="183"/>
-      <c r="J74" s="184"/>
-      <c r="K74" s="166" t="s">
+      <c r="E74" s="128"/>
+      <c r="F74" s="128"/>
+      <c r="G74" s="128"/>
+      <c r="H74" s="128"/>
+      <c r="I74" s="128"/>
+      <c r="J74" s="129"/>
+      <c r="K74" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="L74" s="181"/>
-      <c r="M74" s="167"/>
+      <c r="L74" s="136"/>
+      <c r="M74" s="126"/>
       <c r="N74" s="82" t="s">
         <v>15</v>
       </c>
@@ -4919,16 +4937,16 @@
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A75" s="176"/>
-      <c r="B75" s="130"/>
-      <c r="C75" s="165"/>
-      <c r="D75" s="185"/>
-      <c r="E75" s="186"/>
-      <c r="F75" s="186"/>
-      <c r="G75" s="186"/>
-      <c r="H75" s="186"/>
-      <c r="I75" s="186"/>
-      <c r="J75" s="187"/>
+      <c r="A75" s="122"/>
+      <c r="B75" s="135"/>
+      <c r="C75" s="137"/>
+      <c r="D75" s="130"/>
+      <c r="E75" s="131"/>
+      <c r="F75" s="131"/>
+      <c r="G75" s="131"/>
+      <c r="H75" s="131"/>
+      <c r="I75" s="131"/>
+      <c r="J75" s="132"/>
       <c r="K75" s="80" t="s">
         <v>23</v>
       </c>
@@ -4938,10 +4956,10 @@
       <c r="M75" s="80" t="s">
         <v>91</v>
       </c>
-      <c r="N75" s="166" t="s">
+      <c r="N75" s="125" t="s">
         <v>22</v>
       </c>
-      <c r="O75" s="167"/>
+      <c r="O75" s="126"/>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" s="32">
@@ -5069,17 +5087,17 @@
       </c>
     </row>
     <row r="81" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="126" t="s">
+      <c r="A81" s="118" t="s">
         <v>75</v>
       </c>
-      <c r="B81" s="127"/>
-      <c r="C81" s="127"/>
-      <c r="D81" s="127"/>
-      <c r="E81" s="127"/>
-      <c r="F81" s="127"/>
-      <c r="G81" s="127"/>
-      <c r="H81" s="127"/>
-      <c r="I81" s="171"/>
+      <c r="B81" s="119"/>
+      <c r="C81" s="119"/>
+      <c r="D81" s="119"/>
+      <c r="E81" s="119"/>
+      <c r="F81" s="119"/>
+      <c r="G81" s="119"/>
+      <c r="H81" s="119"/>
+      <c r="I81" s="120"/>
       <c r="J81" s="54" t="s">
         <v>17</v>
       </c>
@@ -5147,48 +5165,48 @@
       <c r="O84" s="6"/>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A85" s="128" t="s">
+      <c r="A85" s="123" t="s">
         <v>33</v>
       </c>
-      <c r="B85" s="128"/>
-      <c r="C85" s="128"/>
-      <c r="D85" s="128"/>
-      <c r="E85" s="128"/>
-      <c r="F85" s="128"/>
-      <c r="G85" s="128"/>
-      <c r="H85" s="128"/>
-      <c r="I85" s="128"/>
-      <c r="J85" s="128"/>
-      <c r="K85" s="128"/>
-      <c r="L85" s="128"/>
-      <c r="M85" s="128"/>
-      <c r="N85" s="128"/>
-      <c r="O85" s="128"/>
+      <c r="B85" s="123"/>
+      <c r="C85" s="123"/>
+      <c r="D85" s="123"/>
+      <c r="E85" s="123"/>
+      <c r="F85" s="123"/>
+      <c r="G85" s="123"/>
+      <c r="H85" s="123"/>
+      <c r="I85" s="123"/>
+      <c r="J85" s="123"/>
+      <c r="K85" s="123"/>
+      <c r="L85" s="123"/>
+      <c r="M85" s="123"/>
+      <c r="N85" s="123"/>
+      <c r="O85" s="123"/>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A86" s="175" t="s">
+      <c r="A86" s="121" t="s">
         <v>36</v>
       </c>
-      <c r="B86" s="129" t="s">
+      <c r="B86" s="134" t="s">
         <v>52</v>
       </c>
-      <c r="C86" s="165" t="s">
+      <c r="C86" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="D86" s="182" t="s">
+      <c r="D86" s="127" t="s">
         <v>40</v>
       </c>
-      <c r="E86" s="183"/>
-      <c r="F86" s="183"/>
-      <c r="G86" s="183"/>
-      <c r="H86" s="183"/>
-      <c r="I86" s="183"/>
-      <c r="J86" s="184"/>
-      <c r="K86" s="166" t="s">
+      <c r="E86" s="128"/>
+      <c r="F86" s="128"/>
+      <c r="G86" s="128"/>
+      <c r="H86" s="128"/>
+      <c r="I86" s="128"/>
+      <c r="J86" s="129"/>
+      <c r="K86" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="L86" s="181"/>
-      <c r="M86" s="167"/>
+      <c r="L86" s="136"/>
+      <c r="M86" s="126"/>
       <c r="N86" s="82" t="s">
         <v>15</v>
       </c>
@@ -5197,16 +5215,16 @@
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A87" s="176"/>
-      <c r="B87" s="130"/>
-      <c r="C87" s="165"/>
-      <c r="D87" s="185"/>
-      <c r="E87" s="186"/>
-      <c r="F87" s="186"/>
-      <c r="G87" s="186"/>
-      <c r="H87" s="186"/>
-      <c r="I87" s="186"/>
-      <c r="J87" s="187"/>
+      <c r="A87" s="122"/>
+      <c r="B87" s="135"/>
+      <c r="C87" s="137"/>
+      <c r="D87" s="130"/>
+      <c r="E87" s="131"/>
+      <c r="F87" s="131"/>
+      <c r="G87" s="131"/>
+      <c r="H87" s="131"/>
+      <c r="I87" s="131"/>
+      <c r="J87" s="132"/>
       <c r="K87" s="80" t="s">
         <v>23</v>
       </c>
@@ -5216,10 +5234,10 @@
       <c r="M87" s="80" t="s">
         <v>91</v>
       </c>
-      <c r="N87" s="166" t="s">
+      <c r="N87" s="125" t="s">
         <v>22</v>
       </c>
-      <c r="O87" s="167"/>
+      <c r="O87" s="126"/>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88" s="32">
@@ -5348,17 +5366,17 @@
       </c>
     </row>
     <row r="93" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="126" t="s">
+      <c r="A93" s="118" t="s">
         <v>75</v>
       </c>
-      <c r="B93" s="127"/>
-      <c r="C93" s="127"/>
-      <c r="D93" s="127"/>
-      <c r="E93" s="127"/>
-      <c r="F93" s="127"/>
-      <c r="G93" s="127"/>
-      <c r="H93" s="127"/>
-      <c r="I93" s="171"/>
+      <c r="B93" s="119"/>
+      <c r="C93" s="119"/>
+      <c r="D93" s="119"/>
+      <c r="E93" s="119"/>
+      <c r="F93" s="119"/>
+      <c r="G93" s="119"/>
+      <c r="H93" s="119"/>
+      <c r="I93" s="120"/>
       <c r="J93" s="54" t="s">
         <v>17</v>
       </c>
@@ -5384,44 +5402,44 @@
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A96" s="128" t="s">
+      <c r="A96" s="123" t="s">
         <v>54</v>
       </c>
-      <c r="B96" s="128"/>
-      <c r="C96" s="128"/>
-      <c r="D96" s="128"/>
-      <c r="E96" s="128"/>
-      <c r="F96" s="128"/>
-      <c r="G96" s="128"/>
-      <c r="H96" s="128"/>
-      <c r="I96" s="128"/>
-      <c r="J96" s="128"/>
-      <c r="K96" s="128"/>
-      <c r="L96" s="128"/>
-      <c r="M96" s="128"/>
-      <c r="N96" s="128"/>
-      <c r="O96" s="128"/>
+      <c r="B96" s="123"/>
+      <c r="C96" s="123"/>
+      <c r="D96" s="123"/>
+      <c r="E96" s="123"/>
+      <c r="F96" s="123"/>
+      <c r="G96" s="123"/>
+      <c r="H96" s="123"/>
+      <c r="I96" s="123"/>
+      <c r="J96" s="123"/>
+      <c r="K96" s="123"/>
+      <c r="L96" s="123"/>
+      <c r="M96" s="123"/>
+      <c r="N96" s="123"/>
+      <c r="O96" s="123"/>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A97" s="175" t="s">
+      <c r="A97" s="121" t="s">
         <v>36</v>
       </c>
-      <c r="B97" s="165" t="s">
+      <c r="B97" s="137" t="s">
         <v>52</v>
       </c>
-      <c r="C97" s="165"/>
-      <c r="D97" s="165"/>
-      <c r="E97" s="165"/>
-      <c r="F97" s="165"/>
-      <c r="G97" s="165"/>
-      <c r="H97" s="165"/>
-      <c r="I97" s="165"/>
-      <c r="J97" s="165"/>
-      <c r="K97" s="181" t="s">
+      <c r="C97" s="137"/>
+      <c r="D97" s="137"/>
+      <c r="E97" s="137"/>
+      <c r="F97" s="137"/>
+      <c r="G97" s="137"/>
+      <c r="H97" s="137"/>
+      <c r="I97" s="137"/>
+      <c r="J97" s="137"/>
+      <c r="K97" s="136" t="s">
         <v>15</v>
       </c>
-      <c r="L97" s="181"/>
-      <c r="M97" s="167"/>
+      <c r="L97" s="136"/>
+      <c r="M97" s="126"/>
       <c r="N97" s="31" t="s">
         <v>15</v>
       </c>
@@ -5430,16 +5448,16 @@
       </c>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A98" s="176"/>
-      <c r="B98" s="165"/>
-      <c r="C98" s="165"/>
-      <c r="D98" s="165"/>
-      <c r="E98" s="165"/>
-      <c r="F98" s="165"/>
-      <c r="G98" s="165"/>
-      <c r="H98" s="165"/>
-      <c r="I98" s="165"/>
-      <c r="J98" s="165"/>
+      <c r="A98" s="122"/>
+      <c r="B98" s="137"/>
+      <c r="C98" s="137"/>
+      <c r="D98" s="137"/>
+      <c r="E98" s="137"/>
+      <c r="F98" s="137"/>
+      <c r="G98" s="137"/>
+      <c r="H98" s="137"/>
+      <c r="I98" s="137"/>
+      <c r="J98" s="137"/>
       <c r="K98" s="81" t="s">
         <v>23</v>
       </c>
@@ -5449,10 +5467,10 @@
       <c r="M98" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="N98" s="166" t="s">
+      <c r="N98" s="125" t="s">
         <v>22</v>
       </c>
-      <c r="O98" s="167"/>
+      <c r="O98" s="126"/>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" s="32">
@@ -5599,17 +5617,17 @@
       </c>
     </row>
     <row r="103" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="126" t="s">
+      <c r="A103" s="118" t="s">
         <v>75</v>
       </c>
-      <c r="B103" s="127"/>
-      <c r="C103" s="127"/>
-      <c r="D103" s="127"/>
-      <c r="E103" s="127"/>
-      <c r="F103" s="127"/>
-      <c r="G103" s="127"/>
-      <c r="H103" s="127"/>
-      <c r="I103" s="171"/>
+      <c r="B103" s="119"/>
+      <c r="C103" s="119"/>
+      <c r="D103" s="119"/>
+      <c r="E103" s="119"/>
+      <c r="F103" s="119"/>
+      <c r="G103" s="119"/>
+      <c r="H103" s="119"/>
+      <c r="I103" s="120"/>
       <c r="J103" s="54" t="s">
         <v>17</v>
       </c>
@@ -5652,44 +5670,44 @@
       <c r="O104" s="41"/>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A105" s="172" t="s">
+      <c r="A105" s="155" t="s">
         <v>87</v>
       </c>
-      <c r="B105" s="173"/>
-      <c r="C105" s="173"/>
-      <c r="D105" s="173"/>
-      <c r="E105" s="173"/>
-      <c r="F105" s="173"/>
-      <c r="G105" s="173"/>
-      <c r="H105" s="173"/>
-      <c r="I105" s="173"/>
-      <c r="J105" s="173"/>
-      <c r="K105" s="173"/>
-      <c r="L105" s="173"/>
-      <c r="M105" s="173"/>
-      <c r="N105" s="173"/>
-      <c r="O105" s="174"/>
+      <c r="B105" s="156"/>
+      <c r="C105" s="156"/>
+      <c r="D105" s="156"/>
+      <c r="E105" s="156"/>
+      <c r="F105" s="156"/>
+      <c r="G105" s="156"/>
+      <c r="H105" s="156"/>
+      <c r="I105" s="156"/>
+      <c r="J105" s="156"/>
+      <c r="K105" s="156"/>
+      <c r="L105" s="156"/>
+      <c r="M105" s="156"/>
+      <c r="N105" s="156"/>
+      <c r="O105" s="157"/>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A106" s="175" t="s">
+      <c r="A106" s="121" t="s">
         <v>36</v>
       </c>
-      <c r="B106" s="165" t="s">
+      <c r="B106" s="137" t="s">
         <v>52</v>
       </c>
-      <c r="C106" s="165"/>
-      <c r="D106" s="165"/>
-      <c r="E106" s="165"/>
-      <c r="F106" s="165"/>
-      <c r="G106" s="165"/>
-      <c r="H106" s="165"/>
-      <c r="I106" s="165"/>
-      <c r="J106" s="165"/>
-      <c r="K106" s="166" t="s">
+      <c r="C106" s="137"/>
+      <c r="D106" s="137"/>
+      <c r="E106" s="137"/>
+      <c r="F106" s="137"/>
+      <c r="G106" s="137"/>
+      <c r="H106" s="137"/>
+      <c r="I106" s="137"/>
+      <c r="J106" s="137"/>
+      <c r="K106" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="L106" s="181"/>
-      <c r="M106" s="167"/>
+      <c r="L106" s="136"/>
+      <c r="M106" s="126"/>
       <c r="N106" s="31" t="s">
         <v>15</v>
       </c>
@@ -5698,16 +5716,16 @@
       </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A107" s="176"/>
-      <c r="B107" s="165"/>
-      <c r="C107" s="165"/>
-      <c r="D107" s="165"/>
-      <c r="E107" s="165"/>
-      <c r="F107" s="165"/>
-      <c r="G107" s="165"/>
-      <c r="H107" s="165"/>
-      <c r="I107" s="165"/>
-      <c r="J107" s="165"/>
+      <c r="A107" s="122"/>
+      <c r="B107" s="137"/>
+      <c r="C107" s="137"/>
+      <c r="D107" s="137"/>
+      <c r="E107" s="137"/>
+      <c r="F107" s="137"/>
+      <c r="G107" s="137"/>
+      <c r="H107" s="137"/>
+      <c r="I107" s="137"/>
+      <c r="J107" s="137"/>
       <c r="K107" s="81" t="s">
         <v>23</v>
       </c>
@@ -5717,10 +5735,10 @@
       <c r="M107" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="N107" s="166" t="s">
+      <c r="N107" s="125" t="s">
         <v>22</v>
       </c>
-      <c r="O107" s="167"/>
+      <c r="O107" s="126"/>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" s="32">
@@ -5867,17 +5885,17 @@
       </c>
     </row>
     <row r="112" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="126" t="s">
+      <c r="A112" s="118" t="s">
         <v>75</v>
       </c>
-      <c r="B112" s="127"/>
-      <c r="C112" s="127"/>
-      <c r="D112" s="127"/>
-      <c r="E112" s="127"/>
-      <c r="F112" s="127"/>
-      <c r="G112" s="127"/>
-      <c r="H112" s="127"/>
-      <c r="I112" s="171"/>
+      <c r="B112" s="119"/>
+      <c r="C112" s="119"/>
+      <c r="D112" s="119"/>
+      <c r="E112" s="119"/>
+      <c r="F112" s="119"/>
+      <c r="G112" s="119"/>
+      <c r="H112" s="119"/>
+      <c r="I112" s="120"/>
       <c r="J112" s="54" t="s">
         <v>17</v>
       </c>
@@ -5903,18 +5921,18 @@
       </c>
     </row>
     <row r="113" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="178" t="s">
+      <c r="A113" s="158" t="s">
         <v>88</v>
       </c>
-      <c r="B113" s="178"/>
-      <c r="C113" s="178"/>
-      <c r="D113" s="178"/>
-      <c r="E113" s="178"/>
-      <c r="F113" s="178"/>
-      <c r="G113" s="178"/>
-      <c r="H113" s="178"/>
-      <c r="I113" s="178"/>
-      <c r="J113" s="178"/>
+      <c r="B113" s="158"/>
+      <c r="C113" s="158"/>
+      <c r="D113" s="158"/>
+      <c r="E113" s="158"/>
+      <c r="F113" s="158"/>
+      <c r="G113" s="158"/>
+      <c r="H113" s="158"/>
+      <c r="I113" s="158"/>
+      <c r="J113" s="158"/>
       <c r="K113" s="41"/>
       <c r="L113" s="42"/>
       <c r="M113" s="42"/>
@@ -5923,11 +5941,11 @@
     </row>
     <row r="114" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="115" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A115" s="168" t="s">
+      <c r="A115" s="152" t="s">
         <v>34</v>
       </c>
-      <c r="B115" s="169"/>
-      <c r="C115" s="170"/>
+      <c r="B115" s="153"/>
+      <c r="C115" s="154"/>
       <c r="D115" s="43"/>
       <c r="E115" s="43"/>
       <c r="F115" s="43"/>
@@ -5958,19 +5976,19 @@
         <f>IFERROR(N29/$N$126*100, 0)</f>
         <v>70.103882335487654</v>
       </c>
-      <c r="E117" s="177" t="s">
+      <c r="E117" s="139" t="s">
         <v>110</v>
       </c>
-      <c r="F117" s="177"/>
-      <c r="G117" s="177"/>
-      <c r="H117" s="177"/>
-      <c r="I117" s="177"/>
-      <c r="J117" s="177"/>
-      <c r="K117" s="177"/>
-      <c r="L117" s="177"/>
-      <c r="M117" s="177"/>
-      <c r="N117" s="177"/>
-      <c r="O117" s="177"/>
+      <c r="F117" s="139"/>
+      <c r="G117" s="139"/>
+      <c r="H117" s="139"/>
+      <c r="I117" s="139"/>
+      <c r="J117" s="139"/>
+      <c r="K117" s="139"/>
+      <c r="L117" s="139"/>
+      <c r="M117" s="139"/>
+      <c r="N117" s="139"/>
+      <c r="O117" s="139"/>
       <c r="P117" s="53"/>
     </row>
     <row r="118" spans="1:16" ht="63" customHeight="1" x14ac:dyDescent="0.3">
@@ -5985,19 +6003,19 @@
         <f>IFERROR(N53/$N$126*100,0)</f>
         <v>9.4531362717739889</v>
       </c>
-      <c r="E118" s="177" t="s">
+      <c r="E118" s="139" t="s">
         <v>86</v>
       </c>
-      <c r="F118" s="177"/>
-      <c r="G118" s="177"/>
-      <c r="H118" s="177"/>
-      <c r="I118" s="177"/>
-      <c r="J118" s="177"/>
-      <c r="K118" s="177"/>
-      <c r="L118" s="177"/>
-      <c r="M118" s="177"/>
-      <c r="N118" s="177"/>
-      <c r="O118" s="177"/>
+      <c r="F118" s="139"/>
+      <c r="G118" s="139"/>
+      <c r="H118" s="139"/>
+      <c r="I118" s="139"/>
+      <c r="J118" s="139"/>
+      <c r="K118" s="139"/>
+      <c r="L118" s="139"/>
+      <c r="M118" s="139"/>
+      <c r="N118" s="139"/>
+      <c r="O118" s="139"/>
     </row>
     <row r="119" spans="1:16" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="47" t="s">
@@ -6011,19 +6029,19 @@
         <f>IFERROR(N69/$N$126*100,0)</f>
         <v>10.442981392738364</v>
       </c>
-      <c r="E119" s="179" t="s">
+      <c r="E119" s="140" t="s">
         <v>112</v>
       </c>
-      <c r="F119" s="179"/>
-      <c r="G119" s="179"/>
-      <c r="H119" s="179"/>
-      <c r="I119" s="179"/>
-      <c r="J119" s="179"/>
-      <c r="K119" s="179"/>
-      <c r="L119" s="179"/>
-      <c r="M119" s="179"/>
-      <c r="N119" s="179"/>
-      <c r="O119" s="179"/>
+      <c r="F119" s="140"/>
+      <c r="G119" s="140"/>
+      <c r="H119" s="140"/>
+      <c r="I119" s="140"/>
+      <c r="J119" s="140"/>
+      <c r="K119" s="140"/>
+      <c r="L119" s="140"/>
+      <c r="M119" s="140"/>
+      <c r="N119" s="140"/>
+      <c r="O119" s="140"/>
     </row>
     <row r="120" spans="1:16" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="47" t="s">
@@ -6037,19 +6055,19 @@
         <f>IFERROR(N81/$N$126*100, 0)</f>
         <v>0</v>
       </c>
-      <c r="E120" s="180" t="s">
+      <c r="E120" s="141" t="s">
         <v>51</v>
       </c>
-      <c r="F120" s="180"/>
-      <c r="G120" s="180"/>
-      <c r="H120" s="180"/>
-      <c r="I120" s="180"/>
-      <c r="J120" s="180"/>
-      <c r="K120" s="180"/>
-      <c r="L120" s="180"/>
-      <c r="M120" s="180"/>
-      <c r="N120" s="180"/>
-      <c r="O120" s="180"/>
+      <c r="F120" s="141"/>
+      <c r="G120" s="141"/>
+      <c r="H120" s="141"/>
+      <c r="I120" s="141"/>
+      <c r="J120" s="141"/>
+      <c r="K120" s="141"/>
+      <c r="L120" s="141"/>
+      <c r="M120" s="141"/>
+      <c r="N120" s="141"/>
+      <c r="O120" s="141"/>
     </row>
     <row r="121" spans="1:16" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="47" t="s">
@@ -6076,38 +6094,38 @@
         <f>IFERROR(N103/$N$126*100, 0)</f>
         <v>10</v>
       </c>
-      <c r="E122" s="179" t="s">
+      <c r="E122" s="140" t="s">
         <v>98</v>
       </c>
-      <c r="F122" s="179"/>
-      <c r="G122" s="179"/>
-      <c r="H122" s="179"/>
-      <c r="I122" s="179"/>
-      <c r="J122" s="179"/>
-      <c r="K122" s="179"/>
-      <c r="L122" s="179"/>
-      <c r="M122" s="179"/>
-      <c r="N122" s="179"/>
-      <c r="O122" s="179"/>
+      <c r="F122" s="140"/>
+      <c r="G122" s="140"/>
+      <c r="H122" s="140"/>
+      <c r="I122" s="140"/>
+      <c r="J122" s="140"/>
+      <c r="K122" s="140"/>
+      <c r="L122" s="140"/>
+      <c r="M122" s="140"/>
+      <c r="N122" s="140"/>
+      <c r="O122" s="140"/>
     </row>
     <row r="124" spans="1:16" ht="18" x14ac:dyDescent="0.35">
-      <c r="A124" s="162" t="s">
+      <c r="A124" s="149" t="s">
         <v>93</v>
       </c>
-      <c r="B124" s="163"/>
-      <c r="C124" s="163"/>
-      <c r="D124" s="163"/>
-      <c r="E124" s="163"/>
-      <c r="F124" s="163"/>
-      <c r="G124" s="163"/>
-      <c r="H124" s="163"/>
-      <c r="I124" s="163"/>
-      <c r="J124" s="163"/>
-      <c r="K124" s="163"/>
-      <c r="L124" s="163"/>
-      <c r="M124" s="163"/>
-      <c r="N124" s="163"/>
-      <c r="O124" s="164"/>
+      <c r="B124" s="150"/>
+      <c r="C124" s="150"/>
+      <c r="D124" s="150"/>
+      <c r="E124" s="150"/>
+      <c r="F124" s="150"/>
+      <c r="G124" s="150"/>
+      <c r="H124" s="150"/>
+      <c r="I124" s="150"/>
+      <c r="J124" s="150"/>
+      <c r="K124" s="150"/>
+      <c r="L124" s="150"/>
+      <c r="M124" s="150"/>
+      <c r="N124" s="150"/>
+      <c r="O124" s="151"/>
     </row>
     <row r="125" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A125" s="6"/>
@@ -6218,22 +6236,22 @@
       <c r="M133" s="51"/>
     </row>
     <row r="134" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C134" s="160"/>
-      <c r="D134" s="160"/>
-      <c r="E134" s="160"/>
-      <c r="F134" s="160"/>
+      <c r="C134" s="138"/>
+      <c r="D134" s="138"/>
+      <c r="E134" s="138"/>
+      <c r="F134" s="138"/>
     </row>
     <row r="135" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C135" s="161"/>
-      <c r="D135" s="161"/>
-      <c r="E135" s="161"/>
-      <c r="F135" s="161"/>
+      <c r="C135" s="148"/>
+      <c r="D135" s="148"/>
+      <c r="E135" s="148"/>
+      <c r="F135" s="148"/>
     </row>
     <row r="136" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C136" s="160"/>
-      <c r="D136" s="160"/>
-      <c r="E136" s="160"/>
-      <c r="F136" s="160"/>
+      <c r="C136" s="138"/>
+      <c r="D136" s="138"/>
+      <c r="E136" s="138"/>
+      <c r="F136" s="138"/>
     </row>
     <row r="139" spans="3:13" ht="18" x14ac:dyDescent="0.3">
       <c r="C139" s="50"/>
@@ -6301,56 +6319,52 @@
       <c r="M143" s="51"/>
     </row>
     <row r="144" spans="3:13" x14ac:dyDescent="0.3">
-      <c r="C144" s="160"/>
-      <c r="D144" s="160"/>
-      <c r="E144" s="160"/>
-      <c r="F144" s="160"/>
+      <c r="C144" s="138"/>
+      <c r="D144" s="138"/>
+      <c r="E144" s="138"/>
+      <c r="F144" s="138"/>
     </row>
   </sheetData>
   <mergeCells count="106">
-    <mergeCell ref="D76:J76"/>
-    <mergeCell ref="A69:I69"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="A57:O57"/>
-    <mergeCell ref="A73:O73"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="N34:O34"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A53:I53"/>
-    <mergeCell ref="D58:J59"/>
-    <mergeCell ref="D60:J60"/>
-    <mergeCell ref="D62:J62"/>
-    <mergeCell ref="K33:M33"/>
-    <mergeCell ref="N59:O59"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="D66:J66"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="D74:J75"/>
-    <mergeCell ref="K74:M74"/>
-    <mergeCell ref="A81:I81"/>
-    <mergeCell ref="A93:I93"/>
-    <mergeCell ref="A103:I103"/>
-    <mergeCell ref="K97:M97"/>
-    <mergeCell ref="K86:M86"/>
-    <mergeCell ref="A85:O85"/>
-    <mergeCell ref="N87:O87"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="A96:O96"/>
-    <mergeCell ref="N98:O98"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="D88:J88"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="D86:J87"/>
-    <mergeCell ref="C134:F134"/>
-    <mergeCell ref="E117:O117"/>
-    <mergeCell ref="E119:O119"/>
-    <mergeCell ref="E120:O120"/>
-    <mergeCell ref="E122:O122"/>
-    <mergeCell ref="D92:J92"/>
-    <mergeCell ref="B97:J98"/>
-    <mergeCell ref="B106:J107"/>
-    <mergeCell ref="K106:M106"/>
+    <mergeCell ref="D77:J77"/>
+    <mergeCell ref="D78:J78"/>
+    <mergeCell ref="D63:J63"/>
+    <mergeCell ref="D65:J65"/>
+    <mergeCell ref="J11:O11"/>
+    <mergeCell ref="J12:O12"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="K58:M58"/>
+    <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A32:O32"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="A14:O14"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D15:E16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="E33:J34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="A3:O3"/>
@@ -6375,45 +6389,49 @@
     <mergeCell ref="A106:A107"/>
     <mergeCell ref="E118:O118"/>
     <mergeCell ref="A113:J113"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="E33:J34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D77:J77"/>
-    <mergeCell ref="D78:J78"/>
-    <mergeCell ref="D63:J63"/>
-    <mergeCell ref="D65:J65"/>
-    <mergeCell ref="J11:O11"/>
-    <mergeCell ref="J12:O12"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="K58:M58"/>
-    <mergeCell ref="A29:F29"/>
-    <mergeCell ref="A32:O32"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="A14:O14"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D15:E16"/>
+    <mergeCell ref="C134:F134"/>
+    <mergeCell ref="E117:O117"/>
+    <mergeCell ref="E119:O119"/>
+    <mergeCell ref="E120:O120"/>
+    <mergeCell ref="E122:O122"/>
+    <mergeCell ref="D92:J92"/>
+    <mergeCell ref="B97:J98"/>
+    <mergeCell ref="B106:J107"/>
+    <mergeCell ref="K106:M106"/>
+    <mergeCell ref="A81:I81"/>
+    <mergeCell ref="A93:I93"/>
+    <mergeCell ref="A103:I103"/>
+    <mergeCell ref="K97:M97"/>
+    <mergeCell ref="K86:M86"/>
+    <mergeCell ref="A85:O85"/>
+    <mergeCell ref="N87:O87"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="A96:O96"/>
+    <mergeCell ref="N98:O98"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="D88:J88"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="D86:J87"/>
+    <mergeCell ref="D76:J76"/>
+    <mergeCell ref="A69:I69"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="A57:O57"/>
+    <mergeCell ref="A73:O73"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A53:I53"/>
+    <mergeCell ref="D58:J59"/>
+    <mergeCell ref="D60:J60"/>
+    <mergeCell ref="D62:J62"/>
+    <mergeCell ref="K33:M33"/>
+    <mergeCell ref="N59:O59"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="D66:J66"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="D74:J75"/>
+    <mergeCell ref="K74:M74"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H17:J28" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -6724,11 +6742,11 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="189" t="s">
+      <c r="A3" s="192" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="190"/>
-      <c r="C3" s="190"/>
+      <c r="B3" s="193"/>
+      <c r="C3" s="193"/>
     </row>
     <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="62" t="s">
@@ -6863,11 +6881,11 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="189" t="s">
+      <c r="A16" s="192" t="s">
         <v>96</v>
       </c>
-      <c r="B16" s="190"/>
-      <c r="C16" s="190"/>
+      <c r="B16" s="193"/>
+      <c r="C16" s="193"/>
     </row>
     <row r="17" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="62" t="s">
@@ -7024,11 +7042,11 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="189" t="s">
+      <c r="A31" s="192" t="s">
         <v>97</v>
       </c>
-      <c r="B31" s="190"/>
-      <c r="C31" s="190"/>
+      <c r="B31" s="193"/>
+      <c r="C31" s="193"/>
     </row>
     <row r="32" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="62" t="s">
@@ -7129,11 +7147,11 @@
       <c r="C41" s="63"/>
     </row>
     <row r="42" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="189" t="s">
+      <c r="A42" s="192" t="s">
         <v>74</v>
       </c>
-      <c r="B42" s="190"/>
-      <c r="C42" s="190"/>
+      <c r="B42" s="193"/>
+      <c r="C42" s="193"/>
     </row>
     <row r="43" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="62">
@@ -7171,11 +7189,11 @@
       <c r="C47" s="63"/>
     </row>
     <row r="48" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="189" t="s">
+      <c r="A48" s="192" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="190"/>
-      <c r="C48" s="190"/>
+      <c r="B48" s="193"/>
+      <c r="C48" s="193"/>
     </row>
     <row r="49" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="62">
@@ -7213,11 +7231,11 @@
       <c r="C53" s="63"/>
     </row>
     <row r="54" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="189" t="s">
+      <c r="A54" s="192" t="s">
         <v>55</v>
       </c>
-      <c r="B54" s="190"/>
-      <c r="C54" s="190"/>
+      <c r="B54" s="193"/>
+      <c r="C54" s="193"/>
     </row>
     <row r="55" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="62">
@@ -7263,11 +7281,11 @@
       <c r="C59" s="63"/>
     </row>
     <row r="60" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="189" t="s">
+      <c r="A60" s="192" t="s">
         <v>58</v>
       </c>
-      <c r="B60" s="190"/>
-      <c r="C60" s="190"/>
+      <c r="B60" s="193"/>
+      <c r="C60" s="193"/>
     </row>
     <row r="61" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="62">
@@ -7307,11 +7325,11 @@
       <c r="C65" s="63"/>
     </row>
     <row r="66" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="191" t="s">
+      <c r="A66" s="196" t="s">
         <v>111</v>
       </c>
-      <c r="B66" s="192"/>
-      <c r="C66" s="192"/>
+      <c r="B66" s="197"/>
+      <c r="C66" s="197"/>
     </row>
     <row r="67" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="64" t="s">
@@ -7377,25 +7395,25 @@
       <c r="C73" s="63"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="189" t="s">
+      <c r="A74" s="192" t="s">
         <v>39</v>
       </c>
-      <c r="B74" s="190"/>
-      <c r="C74" s="190"/>
+      <c r="B74" s="193"/>
+      <c r="C74" s="193"/>
     </row>
     <row r="75" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="B75" s="196"/>
-      <c r="C75" s="197"/>
+      <c r="B75" s="194"/>
+      <c r="C75" s="195"/>
     </row>
     <row r="77" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A77" s="193" t="s">
+      <c r="A77" s="189" t="s">
         <v>46</v>
       </c>
-      <c r="B77" s="193"/>
-      <c r="C77" s="193"/>
+      <c r="B77" s="189"/>
+      <c r="C77" s="189"/>
     </row>
     <row r="78" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A78" s="94" t="s">
@@ -7412,32 +7430,26 @@
       <c r="C79" s="66"/>
     </row>
     <row r="80" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A80" s="194" t="s">
+      <c r="A80" s="190" t="s">
         <v>47</v>
       </c>
-      <c r="B80" s="194"/>
-      <c r="C80" s="194"/>
+      <c r="B80" s="190"/>
+      <c r="C80" s="190"/>
     </row>
     <row r="81" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A81" s="194" t="s">
+      <c r="A81" s="190" t="s">
         <v>114</v>
       </c>
-      <c r="B81" s="194"/>
-      <c r="C81" s="194"/>
+      <c r="B81" s="190"/>
+      <c r="C81" s="190"/>
     </row>
     <row r="82" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A82" s="195"/>
-      <c r="B82" s="195"/>
-      <c r="C82" s="195"/>
+      <c r="A82" s="191"/>
+      <c r="B82" s="191"/>
+      <c r="C82" s="191"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A77:C77"/>
-    <mergeCell ref="A80:C80"/>
-    <mergeCell ref="A81:C81"/>
-    <mergeCell ref="A82:C82"/>
-    <mergeCell ref="A74:C74"/>
-    <mergeCell ref="B75:C75"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="A31:C31"/>
@@ -7446,6 +7458,12 @@
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="A48:C48"/>
     <mergeCell ref="A60:C60"/>
+    <mergeCell ref="A77:C77"/>
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="A81:C81"/>
+    <mergeCell ref="A82:C82"/>
+    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="B75:C75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7467,58 +7485,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="154" t="s">
+      <c r="A1" s="142" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="154"/>
-      <c r="C1" s="154"/>
-      <c r="D1" s="154"/>
-      <c r="E1" s="154"/>
-      <c r="F1" s="154"/>
-      <c r="G1" s="154"/>
-      <c r="H1" s="154"/>
-      <c r="I1" s="154"/>
-      <c r="J1" s="154"/>
-      <c r="K1" s="154"/>
-      <c r="L1" s="154"/>
-      <c r="M1" s="154"/>
-      <c r="N1" s="154"/>
+      <c r="B1" s="142"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
+      <c r="J1" s="142"/>
+      <c r="K1" s="142"/>
+      <c r="L1" s="142"/>
+      <c r="M1" s="142"/>
+      <c r="N1" s="142"/>
     </row>
     <row r="2" spans="1:14" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="155" t="s">
+      <c r="A2" s="143" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="155"/>
-      <c r="C2" s="155"/>
-      <c r="D2" s="155"/>
-      <c r="E2" s="155"/>
-      <c r="F2" s="155"/>
-      <c r="G2" s="155"/>
-      <c r="H2" s="155"/>
-      <c r="I2" s="155"/>
-      <c r="J2" s="155"/>
-      <c r="K2" s="155"/>
-      <c r="L2" s="155"/>
-      <c r="M2" s="155"/>
-      <c r="N2" s="155"/>
+      <c r="B2" s="143"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2" s="143"/>
+      <c r="H2" s="143"/>
+      <c r="I2" s="143"/>
+      <c r="J2" s="143"/>
+      <c r="K2" s="143"/>
+      <c r="L2" s="143"/>
+      <c r="M2" s="143"/>
+      <c r="N2" s="143"/>
     </row>
     <row r="3" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="156" t="s">
+      <c r="A3" s="144" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="156"/>
-      <c r="C3" s="156"/>
-      <c r="D3" s="156"/>
-      <c r="E3" s="156"/>
-      <c r="F3" s="156"/>
-      <c r="G3" s="156"/>
-      <c r="H3" s="156"/>
-      <c r="I3" s="156"/>
-      <c r="J3" s="156"/>
-      <c r="K3" s="156"/>
-      <c r="L3" s="156"/>
-      <c r="M3" s="156"/>
-      <c r="N3" s="156"/>
+      <c r="B3" s="144"/>
+      <c r="C3" s="144"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+      <c r="H3" s="144"/>
+      <c r="I3" s="144"/>
+      <c r="J3" s="144"/>
+      <c r="K3" s="144"/>
+      <c r="L3" s="144"/>
+      <c r="M3" s="144"/>
+      <c r="N3" s="144"/>
     </row>
     <row r="4" spans="1:14" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
@@ -7537,28 +7555,28 @@
       <c r="N4" s="6"/>
     </row>
     <row r="5" spans="1:14" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="152" t="s">
+      <c r="A5" s="166" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="153"/>
-      <c r="C5" s="157"/>
-      <c r="D5" s="158"/>
-      <c r="E5" s="158"/>
-      <c r="F5" s="158"/>
-      <c r="G5" s="158"/>
-      <c r="H5" s="158"/>
-      <c r="I5" s="158"/>
-      <c r="J5" s="158"/>
-      <c r="K5" s="158"/>
-      <c r="L5" s="158"/>
-      <c r="M5" s="158"/>
-      <c r="N5" s="159"/>
+      <c r="B5" s="167"/>
+      <c r="C5" s="145"/>
+      <c r="D5" s="146"/>
+      <c r="E5" s="146"/>
+      <c r="F5" s="146"/>
+      <c r="G5" s="146"/>
+      <c r="H5" s="146"/>
+      <c r="I5" s="146"/>
+      <c r="J5" s="146"/>
+      <c r="K5" s="146"/>
+      <c r="L5" s="146"/>
+      <c r="M5" s="146"/>
+      <c r="N5" s="147"/>
     </row>
     <row r="6" spans="1:14" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="152" t="s">
+      <c r="A6" s="166" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="153"/>
+      <c r="B6" s="167"/>
       <c r="C6" s="69"/>
       <c r="D6" s="70"/>
       <c r="E6" s="70"/>
@@ -7573,40 +7591,40 @@
       <c r="N6" s="71"/>
     </row>
     <row r="7" spans="1:14" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="152" t="s">
+      <c r="A7" s="166" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="153"/>
-      <c r="C7" s="157"/>
-      <c r="D7" s="158"/>
-      <c r="E7" s="158"/>
-      <c r="F7" s="158"/>
-      <c r="G7" s="158"/>
-      <c r="H7" s="158"/>
-      <c r="I7" s="158"/>
-      <c r="J7" s="158"/>
-      <c r="K7" s="158"/>
-      <c r="L7" s="158"/>
-      <c r="M7" s="158"/>
-      <c r="N7" s="159"/>
+      <c r="B7" s="167"/>
+      <c r="C7" s="145"/>
+      <c r="D7" s="146"/>
+      <c r="E7" s="146"/>
+      <c r="F7" s="146"/>
+      <c r="G7" s="146"/>
+      <c r="H7" s="146"/>
+      <c r="I7" s="146"/>
+      <c r="J7" s="146"/>
+      <c r="K7" s="146"/>
+      <c r="L7" s="146"/>
+      <c r="M7" s="146"/>
+      <c r="N7" s="147"/>
     </row>
     <row r="8" spans="1:14" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="152" t="s">
+      <c r="A8" s="166" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="153"/>
-      <c r="C8" s="157"/>
-      <c r="D8" s="158"/>
-      <c r="E8" s="158"/>
-      <c r="F8" s="158"/>
-      <c r="G8" s="158"/>
-      <c r="H8" s="158"/>
-      <c r="I8" s="158"/>
-      <c r="J8" s="158"/>
-      <c r="K8" s="158"/>
-      <c r="L8" s="158"/>
-      <c r="M8" s="158"/>
-      <c r="N8" s="159"/>
+      <c r="B8" s="167"/>
+      <c r="C8" s="145"/>
+      <c r="D8" s="146"/>
+      <c r="E8" s="146"/>
+      <c r="F8" s="146"/>
+      <c r="G8" s="146"/>
+      <c r="H8" s="146"/>
+      <c r="I8" s="146"/>
+      <c r="J8" s="146"/>
+      <c r="K8" s="146"/>
+      <c r="L8" s="146"/>
+      <c r="M8" s="146"/>
+      <c r="N8" s="147"/>
     </row>
     <row r="9" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
@@ -7625,66 +7643,66 @@
       <c r="N9" s="6"/>
     </row>
     <row r="12" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="172" t="s">
+      <c r="A12" s="155" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="173"/>
-      <c r="C12" s="173"/>
-      <c r="D12" s="173"/>
-      <c r="E12" s="173"/>
-      <c r="F12" s="173"/>
-      <c r="G12" s="173"/>
-      <c r="H12" s="173"/>
-      <c r="I12" s="173"/>
-      <c r="J12" s="173"/>
-      <c r="K12" s="173"/>
-      <c r="L12" s="173"/>
-      <c r="M12" s="173"/>
-      <c r="N12" s="174"/>
+      <c r="B12" s="156"/>
+      <c r="C12" s="156"/>
+      <c r="D12" s="156"/>
+      <c r="E12" s="156"/>
+      <c r="F12" s="156"/>
+      <c r="G12" s="156"/>
+      <c r="H12" s="156"/>
+      <c r="I12" s="156"/>
+      <c r="J12" s="156"/>
+      <c r="K12" s="156"/>
+      <c r="L12" s="156"/>
+      <c r="M12" s="156"/>
+      <c r="N12" s="157"/>
     </row>
     <row r="13" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="175" t="s">
+      <c r="A13" s="121" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="129" t="s">
+      <c r="B13" s="134" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="129" t="s">
+      <c r="C13" s="134" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="182" t="s">
+      <c r="D13" s="127" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="183"/>
-      <c r="F13" s="183"/>
-      <c r="G13" s="183"/>
-      <c r="H13" s="183"/>
-      <c r="I13" s="183"/>
-      <c r="J13" s="184"/>
-      <c r="K13" s="210" t="s">
+      <c r="E13" s="128"/>
+      <c r="F13" s="128"/>
+      <c r="G13" s="128"/>
+      <c r="H13" s="128"/>
+      <c r="I13" s="128"/>
+      <c r="J13" s="129"/>
+      <c r="K13" s="198" t="s">
         <v>15</v>
       </c>
-      <c r="L13" s="211"/>
-      <c r="M13" s="210" t="s">
+      <c r="L13" s="199"/>
+      <c r="M13" s="198" t="s">
         <v>16</v>
       </c>
-      <c r="N13" s="211"/>
+      <c r="N13" s="199"/>
     </row>
     <row r="14" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="176"/>
-      <c r="B14" s="130"/>
-      <c r="C14" s="130"/>
-      <c r="D14" s="185"/>
-      <c r="E14" s="186"/>
-      <c r="F14" s="186"/>
-      <c r="G14" s="186"/>
-      <c r="H14" s="186"/>
-      <c r="I14" s="186"/>
-      <c r="J14" s="187"/>
-      <c r="K14" s="212"/>
-      <c r="L14" s="213"/>
-      <c r="M14" s="212"/>
-      <c r="N14" s="213"/>
+      <c r="A14" s="122"/>
+      <c r="B14" s="135"/>
+      <c r="C14" s="135"/>
+      <c r="D14" s="130"/>
+      <c r="E14" s="131"/>
+      <c r="F14" s="131"/>
+      <c r="G14" s="131"/>
+      <c r="H14" s="131"/>
+      <c r="I14" s="131"/>
+      <c r="J14" s="132"/>
+      <c r="K14" s="200"/>
+      <c r="L14" s="201"/>
+      <c r="M14" s="200"/>
+      <c r="N14" s="201"/>
     </row>
     <row r="15" spans="1:14" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="68">
@@ -7692,49 +7710,49 @@
       </c>
       <c r="B15" s="21"/>
       <c r="C15" s="33"/>
-      <c r="D15" s="218"/>
-      <c r="E15" s="218"/>
-      <c r="F15" s="218"/>
-      <c r="G15" s="218"/>
-      <c r="H15" s="218"/>
-      <c r="I15" s="218"/>
-      <c r="J15" s="218"/>
-      <c r="K15" s="208"/>
-      <c r="L15" s="209"/>
-      <c r="M15" s="214">
+      <c r="D15" s="211"/>
+      <c r="E15" s="211"/>
+      <c r="F15" s="211"/>
+      <c r="G15" s="211"/>
+      <c r="H15" s="211"/>
+      <c r="I15" s="211"/>
+      <c r="J15" s="211"/>
+      <c r="K15" s="205"/>
+      <c r="L15" s="206"/>
+      <c r="M15" s="207">
         <f>K15/Budget!D12</f>
         <v>0</v>
       </c>
-      <c r="N15" s="215" t="e">
+      <c r="N15" s="208" t="e">
         <f>M15/$D$12</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="16" spans="1:14" s="4" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="219" t="s">
+      <c r="A16" s="212" t="s">
         <v>117</v>
       </c>
-      <c r="B16" s="219"/>
-      <c r="C16" s="219"/>
-      <c r="D16" s="219"/>
-      <c r="E16" s="219"/>
-      <c r="F16" s="219"/>
-      <c r="G16" s="219"/>
-      <c r="H16" s="219"/>
-      <c r="I16" s="219"/>
+      <c r="B16" s="212"/>
+      <c r="C16" s="212"/>
+      <c r="D16" s="212"/>
+      <c r="E16" s="212"/>
+      <c r="F16" s="212"/>
+      <c r="G16" s="212"/>
+      <c r="H16" s="212"/>
+      <c r="I16" s="212"/>
       <c r="J16" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="K16" s="216">
+      <c r="K16" s="209">
         <f>K15</f>
         <v>0</v>
       </c>
-      <c r="L16" s="217"/>
-      <c r="M16" s="216">
+      <c r="L16" s="210"/>
+      <c r="M16" s="209">
         <f>M15</f>
         <v>0</v>
       </c>
-      <c r="N16" s="217"/>
+      <c r="N16" s="210"/>
     </row>
     <row r="17" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="73"/>
@@ -7785,148 +7803,148 @@
       <c r="N19"/>
     </row>
     <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="172" t="s">
+      <c r="A20" s="155" t="s">
         <v>84</v>
       </c>
-      <c r="B20" s="173"/>
-      <c r="C20" s="173"/>
-      <c r="D20" s="173"/>
-      <c r="E20" s="173"/>
-      <c r="F20" s="173"/>
-      <c r="G20" s="173"/>
-      <c r="H20" s="173"/>
-      <c r="I20" s="173"/>
-      <c r="J20" s="173"/>
-      <c r="K20" s="173"/>
-      <c r="L20" s="173"/>
-      <c r="M20" s="173"/>
-      <c r="N20" s="174"/>
+      <c r="B20" s="156"/>
+      <c r="C20" s="156"/>
+      <c r="D20" s="156"/>
+      <c r="E20" s="156"/>
+      <c r="F20" s="156"/>
+      <c r="G20" s="156"/>
+      <c r="H20" s="156"/>
+      <c r="I20" s="156"/>
+      <c r="J20" s="156"/>
+      <c r="K20" s="156"/>
+      <c r="L20" s="156"/>
+      <c r="M20" s="156"/>
+      <c r="N20" s="157"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="199"/>
-      <c r="B21" s="200"/>
-      <c r="C21" s="201"/>
-      <c r="D21" s="205" t="s">
+      <c r="A21" s="214"/>
+      <c r="B21" s="215"/>
+      <c r="C21" s="216"/>
+      <c r="D21" s="202" t="s">
         <v>83</v>
       </c>
-      <c r="E21" s="206"/>
-      <c r="F21" s="206"/>
-      <c r="G21" s="206"/>
-      <c r="H21" s="206"/>
-      <c r="I21" s="206"/>
-      <c r="J21" s="206"/>
-      <c r="K21" s="206"/>
-      <c r="L21" s="206"/>
-      <c r="M21" s="206"/>
-      <c r="N21" s="207"/>
+      <c r="E21" s="203"/>
+      <c r="F21" s="203"/>
+      <c r="G21" s="203"/>
+      <c r="H21" s="203"/>
+      <c r="I21" s="203"/>
+      <c r="J21" s="203"/>
+      <c r="K21" s="203"/>
+      <c r="L21" s="203"/>
+      <c r="M21" s="203"/>
+      <c r="N21" s="204"/>
     </row>
     <row r="22" spans="1:14" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="203" t="s">
+      <c r="A22" s="218" t="s">
         <v>104</v>
       </c>
-      <c r="B22" s="203"/>
-      <c r="C22" s="203"/>
-      <c r="D22" s="204"/>
-      <c r="E22" s="204"/>
-      <c r="F22" s="204"/>
-      <c r="G22" s="204"/>
-      <c r="H22" s="204"/>
-      <c r="I22" s="204"/>
-      <c r="J22" s="204"/>
-      <c r="K22" s="204"/>
-      <c r="L22" s="204"/>
-      <c r="M22" s="204"/>
-      <c r="N22" s="204"/>
+      <c r="B22" s="218"/>
+      <c r="C22" s="218"/>
+      <c r="D22" s="219"/>
+      <c r="E22" s="219"/>
+      <c r="F22" s="219"/>
+      <c r="G22" s="219"/>
+      <c r="H22" s="219"/>
+      <c r="I22" s="219"/>
+      <c r="J22" s="219"/>
+      <c r="K22" s="219"/>
+      <c r="L22" s="219"/>
+      <c r="M22" s="219"/>
+      <c r="N22" s="219"/>
     </row>
     <row r="23" spans="1:14" ht="62.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="203" t="s">
+      <c r="A23" s="218" t="s">
         <v>115</v>
       </c>
-      <c r="B23" s="203"/>
-      <c r="C23" s="203"/>
-      <c r="D23" s="204"/>
-      <c r="E23" s="204"/>
-      <c r="F23" s="204"/>
-      <c r="G23" s="204"/>
-      <c r="H23" s="204"/>
-      <c r="I23" s="204"/>
-      <c r="J23" s="204"/>
-      <c r="K23" s="204"/>
-      <c r="L23" s="204"/>
-      <c r="M23" s="204"/>
-      <c r="N23" s="204"/>
+      <c r="B23" s="218"/>
+      <c r="C23" s="218"/>
+      <c r="D23" s="219"/>
+      <c r="E23" s="219"/>
+      <c r="F23" s="219"/>
+      <c r="G23" s="219"/>
+      <c r="H23" s="219"/>
+      <c r="I23" s="219"/>
+      <c r="J23" s="219"/>
+      <c r="K23" s="219"/>
+      <c r="L23" s="219"/>
+      <c r="M23" s="219"/>
+      <c r="N23" s="219"/>
     </row>
     <row r="24" spans="1:14" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="198" t="s">
+      <c r="A24" s="213" t="s">
         <v>105</v>
       </c>
-      <c r="B24" s="198"/>
-      <c r="C24" s="198"/>
-      <c r="D24" s="202"/>
-      <c r="E24" s="202"/>
-      <c r="F24" s="202"/>
-      <c r="G24" s="202"/>
-      <c r="H24" s="202"/>
-      <c r="I24" s="202"/>
-      <c r="J24" s="202"/>
-      <c r="K24" s="202"/>
-      <c r="L24" s="202"/>
-      <c r="M24" s="202"/>
-      <c r="N24" s="202"/>
+      <c r="B24" s="213"/>
+      <c r="C24" s="213"/>
+      <c r="D24" s="217"/>
+      <c r="E24" s="217"/>
+      <c r="F24" s="217"/>
+      <c r="G24" s="217"/>
+      <c r="H24" s="217"/>
+      <c r="I24" s="217"/>
+      <c r="J24" s="217"/>
+      <c r="K24" s="217"/>
+      <c r="L24" s="217"/>
+      <c r="M24" s="217"/>
+      <c r="N24" s="217"/>
     </row>
     <row r="25" spans="1:14" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="203" t="s">
+      <c r="A25" s="218" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="203"/>
-      <c r="C25" s="203"/>
-      <c r="D25" s="202"/>
-      <c r="E25" s="202"/>
-      <c r="F25" s="202"/>
-      <c r="G25" s="202"/>
-      <c r="H25" s="202"/>
-      <c r="I25" s="202"/>
-      <c r="J25" s="202"/>
-      <c r="K25" s="202"/>
-      <c r="L25" s="202"/>
-      <c r="M25" s="202"/>
-      <c r="N25" s="202"/>
+      <c r="B25" s="218"/>
+      <c r="C25" s="218"/>
+      <c r="D25" s="217"/>
+      <c r="E25" s="217"/>
+      <c r="F25" s="217"/>
+      <c r="G25" s="217"/>
+      <c r="H25" s="217"/>
+      <c r="I25" s="217"/>
+      <c r="J25" s="217"/>
+      <c r="K25" s="217"/>
+      <c r="L25" s="217"/>
+      <c r="M25" s="217"/>
+      <c r="N25" s="217"/>
     </row>
     <row r="26" spans="1:14" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="198" t="s">
+      <c r="A26" s="213" t="s">
         <v>116</v>
       </c>
-      <c r="B26" s="198"/>
-      <c r="C26" s="198"/>
-      <c r="D26" s="202"/>
-      <c r="E26" s="202"/>
-      <c r="F26" s="202"/>
-      <c r="G26" s="202"/>
-      <c r="H26" s="202"/>
-      <c r="I26" s="202"/>
-      <c r="J26" s="202"/>
-      <c r="K26" s="202"/>
-      <c r="L26" s="202"/>
-      <c r="M26" s="202"/>
-      <c r="N26" s="202"/>
+      <c r="B26" s="213"/>
+      <c r="C26" s="213"/>
+      <c r="D26" s="217"/>
+      <c r="E26" s="217"/>
+      <c r="F26" s="217"/>
+      <c r="G26" s="217"/>
+      <c r="H26" s="217"/>
+      <c r="I26" s="217"/>
+      <c r="J26" s="217"/>
+      <c r="K26" s="217"/>
+      <c r="L26" s="217"/>
+      <c r="M26" s="217"/>
+      <c r="N26" s="217"/>
     </row>
     <row r="27" spans="1:14" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="198" t="s">
+      <c r="A27" s="213" t="s">
         <v>103</v>
       </c>
-      <c r="B27" s="198"/>
-      <c r="C27" s="198"/>
-      <c r="D27" s="202"/>
-      <c r="E27" s="202"/>
-      <c r="F27" s="202"/>
-      <c r="G27" s="202"/>
-      <c r="H27" s="202"/>
-      <c r="I27" s="202"/>
-      <c r="J27" s="202"/>
-      <c r="K27" s="202"/>
-      <c r="L27" s="202"/>
-      <c r="M27" s="202"/>
-      <c r="N27" s="202"/>
+      <c r="B27" s="213"/>
+      <c r="C27" s="213"/>
+      <c r="D27" s="217"/>
+      <c r="E27" s="217"/>
+      <c r="F27" s="217"/>
+      <c r="G27" s="217"/>
+      <c r="H27" s="217"/>
+      <c r="I27" s="217"/>
+      <c r="J27" s="217"/>
+      <c r="K27" s="217"/>
+      <c r="L27" s="217"/>
+      <c r="M27" s="217"/>
+      <c r="N27" s="217"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="76"/>
@@ -8030,31 +8048,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="A12:N12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:J14"/>
-    <mergeCell ref="K13:L14"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:N8"/>
-    <mergeCell ref="A3:N3"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="A2:N2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:N5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:N7"/>
-    <mergeCell ref="A20:N20"/>
-    <mergeCell ref="D21:N21"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M13:N14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="D15:J15"/>
-    <mergeCell ref="A16:I16"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="D25:N25"/>
@@ -8068,6 +8061,31 @@
     <mergeCell ref="D22:N22"/>
     <mergeCell ref="D23:N23"/>
     <mergeCell ref="D24:N24"/>
+    <mergeCell ref="A20:N20"/>
+    <mergeCell ref="D21:N21"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M13:N14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="D15:J15"/>
+    <mergeCell ref="A16:I16"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:N8"/>
+    <mergeCell ref="A3:N3"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:N5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:N7"/>
+    <mergeCell ref="A12:N12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:J14"/>
+    <mergeCell ref="K13:L14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>